<commit_message>
FRATURE: Credit by Purpose
</commit_message>
<xml_diff>
--- a/src/businessConfidenceBySector/assets/report.xlsx
+++ b/src/businessConfidenceBySector/assets/report.xlsx
@@ -49,7 +49,7 @@
     <t>No</t>
   </si>
   <si>
-    <t>Invalid pdf page, the data contained by pdf dois not look like credit-by-purpose data.</t>
+    <t>Date in the credit-by-purpose table could not be processed. It could be a problem format from header table row or column.</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
         <v>11</v>
       </c>
       <c r="G4">
-        <v>44854.4893569285</v>
+        <v>44854.92500156078</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FEATURE: Credit by Purpose
</commit_message>
<xml_diff>
--- a/src/businessConfidenceBySector/assets/report.xlsx
+++ b/src/businessConfidenceBySector/assets/report.xlsx
@@ -49,7 +49,7 @@
     <t>No</t>
   </si>
   <si>
-    <t>Date in the credit-by-purpose table could not be processed. It could be a problem format from header table row or column.</t>
+    <t>Database failed to get By Sector Business Confidence indicator update date</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
         <v>11</v>
       </c>
       <c r="G4">
-        <v>44854.92500156078</v>
+        <v>44855.71691344741</v>
       </c>
     </row>
   </sheetData>

</xml_diff>